<commit_message>
update Sprint 2 Day 2
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -70,9 +70,6 @@
     <t>send information</t>
   </si>
   <si>
-    <t>Future</t>
-  </si>
-  <si>
     <t>get information from user to database and return desired values</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Link array to UI</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -533,11 +532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="219556792"/>
-        <c:axId val="220699104"/>
+        <c:axId val="207761760"/>
+        <c:axId val="207047600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="219556792"/>
+        <c:axId val="207761760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,7 +578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220699104"/>
+        <c:crossAx val="207047600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -587,7 +586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220699104"/>
+        <c:axId val="207047600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219556792"/>
+        <c:crossAx val="207761760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -652,7 +651,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -945,11 +943,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="455713808"/>
-        <c:axId val="455714200"/>
+        <c:axId val="207049952"/>
+        <c:axId val="207052696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="455713808"/>
+        <c:axId val="207049952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -991,7 +989,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455714200"/>
+        <c:crossAx val="207052696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -999,7 +997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455714200"/>
+        <c:axId val="207052696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455713808"/>
+        <c:crossAx val="207049952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2555,7 +2553,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2578,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2590,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2604,16 +2602,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -2627,16 +2625,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>8</v>
@@ -2651,16 +2649,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
@@ -2675,16 +2673,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>12</v>
@@ -2699,17 +2697,19 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
       <c r="F6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -2718,20 +2718,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -2740,22 +2742,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -2769,7 +2771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2783,31 +2785,31 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -2818,7 +2820,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="7">
         <v>2</v>
@@ -2847,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="7">
         <v>6</v>
@@ -2876,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="7">
         <v>4</v>
@@ -2975,7 +2977,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6">
         <f>SUM(C2:C9)</f>
@@ -3008,7 +3010,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5">
         <f>SUM(C2:C9)</f>
@@ -3052,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3066,31 +3068,31 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -3101,7 +3103,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7">
         <v>2</v>
@@ -3109,7 +3111,9 @@
       <c r="D2" s="7">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -3117,29 +3121,41 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="A4" s="7">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -3202,64 +3218,64 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6">
         <f>SUM(C2:C9)</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" ref="D11:I11" si="0">C11-SUM(D2:D9)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5">
         <f>SUM(C2:C9)</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" ref="D12:I12" si="1">C12-($C$12/6)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update backlog sprint 2 day 3
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -363,6 +363,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -548,11 +549,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="319789536"/>
-        <c:axId val="319789920"/>
+        <c:axId val="239344616"/>
+        <c:axId val="240263240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319789536"/>
+        <c:axId val="239344616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319789920"/>
+        <c:crossAx val="240263240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -602,7 +603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319789920"/>
+        <c:axId val="240263240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319789536"/>
+        <c:crossAx val="239344616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,6 +668,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -959,11 +961,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361502904"/>
-        <c:axId val="361503288"/>
+        <c:axId val="240265200"/>
+        <c:axId val="240262848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361502904"/>
+        <c:axId val="240265200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361503288"/>
+        <c:crossAx val="240262848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1013,7 +1015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361503288"/>
+        <c:axId val="240262848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361502904"/>
+        <c:crossAx val="240265200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2568,7 +2570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3104,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,7 +3166,9 @@
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -3185,7 +3189,9 @@
       <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <v>5</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -3206,7 +3212,9 @@
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -3284,19 +3292,19 @@
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update backlog sprint 2 day 5
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\TVTrackr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Product" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sprint 1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sprint 2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Product" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -181,38 +186,20 @@
     <t>Link array to UI</t>
   </si>
   <si>
-    <t>Android Studio Tutorial Videos</t>
+    <t>Android Studio Tutorial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -228,27 +215,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -296,119 +267,59 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CC33"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 7" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Accent6" xfId="21" builtinId="54" customBuiltin="true"/>
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -467,14 +378,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -486,7 +416,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400">
+              <a:rPr lang="en-US" sz="1400">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -498,11 +428,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="1"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -518,12 +451,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
+                <a:srgbClr val="5B9BD5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -533,17 +463,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
+                <a:srgbClr val="5B9BD5"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -592,12 +536,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ed7d31"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -607,17 +548,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -629,19 +584,19 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.3333333333333</c:v>
+                  <c:v>13.333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.6666666666667</c:v>
+                  <c:v>10.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.33333333333334</c:v>
+                  <c:v>5.3333333333333357</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.66666666666667</c:v>
+                  <c:v>2.6666666666666692</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -655,12 +610,9 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffffff"/>
-            </a:solidFill>
             <a:ln w="19080">
               <a:solidFill>
-                <a:srgbClr val="ffffff"/>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -676,6 +628,14 @@
           </c:marker>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -683,17 +643,13 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:upDownBars>
-          <c:gapWidth val="150"/>
-          <c:upBars/>
-          <c:downBars/>
-        </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="17952530"/>
-        <c:axId val="32255655"/>
+        <c:smooth val="0"/>
+        <c:axId val="373346320"/>
+        <c:axId val="373343968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17952530"/>
+        <c:axId val="373346320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,19 +661,20 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="32255655"/>
+        <c:crossAx val="373343968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32255655"/>
+        <c:axId val="373343968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,12 +684,13 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -741,8 +699,9 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17952530"/>
+        <c:crossAx val="373346320"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -753,6 +712,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -762,29 +726,114 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 2 Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.9358705161854772E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.61498432487605714"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -800,33 +849,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ee4000"/>
-              </a:solidFill>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'Sprint 2'!$C$11:$I$11</c:f>
@@ -834,25 +873,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,33 +913,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ee4000"/>
-              </a:solidFill>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'Sprint 2'!$C$12:$I$12</c:f>
@@ -908,22 +937,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.6666666666667</c:v>
+                  <c:v>18.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.3333333333333</c:v>
+                  <c:v>14.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.66666666666667</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.33333333333333</c:v>
+                  <c:v>3.6666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -933,47 +962,70 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:upDownBars>
-          <c:gapWidth val="150"/>
-          <c:upBars/>
-          <c:downBars/>
-        </c:upDownBars>
-        <c:marker val="1"/>
-        <c:axId val="7699828"/>
-        <c:axId val="9575396"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="411996032"/>
+        <c:axId val="411999952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7699828"/>
+        <c:axId val="411996032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
-        <c:crossAx val="9575396"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411999952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9575396"/>
+        <c:axId val="411999952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,60 +1033,674 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:majorTickMark val="out"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
+          <a:noFill/>
           <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
+            <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
-        <c:crossAx val="7699828"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411996032"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln>
-      <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1048,14 +1714,14 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="988920" y="2372400"/>
-        <a:ext cx="4983480" cy="2742840"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1069,28 +1735,28 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>1802424</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>13189</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>124200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>300240</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>432289</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>89389</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="923040" y="2454480"/>
-        <a:ext cx="5753520" cy="3238560"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1103,32 +1769,290 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.56632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="15.28515625"/>
+    <col min="4" max="4" width="18.5703125"/>
+    <col min="5" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="12.5703125"/>
+    <col min="7" max="7" width="26.42578125"/>
+    <col min="8" max="8" width="11"/>
+    <col min="9" max="9" width="17.5703125"/>
+    <col min="10" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1154,31 +2078,31 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1190,7 +2114,7 @@
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1201,8 +2125,8 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1214,7 +2138,7 @@
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1225,8 +2149,8 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1238,7 +2162,7 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1249,8 +2173,8 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1262,7 +2186,7 @@
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1273,8 +2197,8 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1286,7 +2210,7 @@
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1297,8 +2221,8 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1310,7 +2234,7 @@
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1321,8 +2245,8 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1338,8 +2262,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1356,38 +2280,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="12.42578125"/>
+    <col min="2" max="2" width="30.85546875"/>
+    <col min="3" max="3" width="14.7109375"/>
+    <col min="4" max="4" width="8.7109375"/>
+    <col min="5" max="5" width="17.42578125"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1419,123 +2335,123 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="4">
         <v>0</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="I2" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="4">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="4">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="4">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="4">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="4">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1546,7 +2462,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1557,7 +2473,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1568,7 +2484,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1579,109 +2495,101 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="7" t="n">
-        <f aca="false">SUM(C2:C9)</f>
+      <c r="C11" s="7">
+        <f>SUM(C2:C9)</f>
         <v>16</v>
       </c>
-      <c r="D11" s="7" t="n">
-        <f aca="false">C11-SUM(D2:D9)</f>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11:I11" si="0">C11-SUM(D2:D9)</f>
         <v>13</v>
       </c>
-      <c r="E11" s="7" t="n">
-        <f aca="false">D11-SUM(E2:E9)</f>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F11" s="7" t="n">
-        <f aca="false">E11-SUM(F2:F9)</f>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11" s="7" t="n">
-        <f aca="false">F11-SUM(G2:G9)</f>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H11" s="7" t="n">
-        <f aca="false">G11-SUM(H2:H9)</f>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I11" s="7" t="n">
-        <f aca="false">H11-SUM(I2:I9)</f>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="9" t="n">
-        <f aca="false">SUM(C2:C9)</f>
+      <c r="C12" s="9">
+        <f>SUM(C2:C9)</f>
         <v>16</v>
       </c>
-      <c r="D12" s="9" t="n">
-        <f aca="false">C12-($C$12/6)</f>
-        <v>13.3333333333333</v>
-      </c>
-      <c r="E12" s="9" t="n">
-        <f aca="false">D12-($C$12/6)</f>
-        <v>10.6666666666667</v>
-      </c>
-      <c r="F12" s="9" t="n">
-        <f aca="false">E12-($C$12/6)</f>
-        <v>8</v>
-      </c>
-      <c r="G12" s="9" t="n">
-        <f aca="false">F12-($C$12/6)</f>
-        <v>5.33333333333334</v>
-      </c>
-      <c r="H12" s="9" t="n">
-        <f aca="false">G12-($C$12/6)</f>
-        <v>2.66666666666667</v>
-      </c>
-      <c r="I12" s="9" t="n">
-        <f aca="false">H12-($C$12/6)</f>
+      <c r="D12" s="9">
+        <f t="shared" ref="D12:I12" si="1">C12-($C$12/6)</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="1"/>
+        <v>10.666666666666668</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>5.3333333333333357</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666692</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="12.42578125"/>
+    <col min="2" max="2" width="30.85546875"/>
+    <col min="3" max="3" width="14.7109375"/>
+    <col min="4" max="4" width="8.7109375"/>
+    <col min="5" max="5" width="17.42578125"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1715,72 +2623,74 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="10" t="n">
-        <f aca="false">C2-SUM(D2,E2,F2,G2,H2,I2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="J2" s="10">
+        <f t="shared" ref="J2:J9" si="0">C2-SUM(D2,E2,F2,G2,H2,I2)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="11" t="n">
-        <f aca="false">C3-SUM(D3,E3,F3,G3,H3,I3)</f>
+      <c r="J3" s="10">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="4">
         <v>6</v>
       </c>
       <c r="D4" s="4"/>
@@ -1789,35 +2699,37 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="11" t="n">
-        <f aca="false">C4-SUM(D4,E4,F4,G4,H4,I4)</f>
+      <c r="J4" s="10">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>2</v>
+      <c r="C5" s="4">
+        <v>4</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="10" t="n">
-        <f aca="false">C5-SUM(D5,E5,F5,G5,H5,I5)</f>
+      <c r="J5" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1827,12 +2739,12 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="11" t="n">
-        <f aca="false">C6-SUM(D6,E6,F6,G6,H6,I6)</f>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1842,12 +2754,12 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="11" t="n">
-        <f aca="false">C7-SUM(D7,E7,F7,G7,H7,I7)</f>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1857,12 +2769,12 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="11" t="n">
-        <f aca="false">C8-SUM(D8,E8,F8,G8,H8,I8)</f>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1872,88 +2784,83 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="11" t="n">
-        <f aca="false">C9-SUM(D9,E9,F9,G9,H9,I9)</f>
+      <c r="J9" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="7" t="n">
-        <f aca="false">SUM(C2:C9)</f>
-        <v>20</v>
-      </c>
-      <c r="D11" s="7" t="n">
-        <f aca="false">C11-SUM(D2:D9)</f>
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="n">
-        <f aca="false">D11-SUM(E2:E9)</f>
-        <v>16</v>
-      </c>
-      <c r="F11" s="7" t="n">
-        <f aca="false">E11-SUM(F2:F9)</f>
+      <c r="C11" s="7">
+        <f>SUM(C2:C9)</f>
+        <v>22</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11:I11" si="1">C11-SUM(D2:D9)</f>
+        <v>18</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G11" s="7" t="n">
-        <f aca="false">F11-SUM(G2:G9)</f>
-        <v>9</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <f aca="false">G11-SUM(H2:H9)</f>
-        <v>9</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <f aca="false">H11-SUM(I2:I9)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="9" t="n">
-        <f aca="false">SUM(C2:C9)</f>
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="n">
-        <f aca="false">C12-($C$12/6)</f>
-        <v>16.6666666666667</v>
-      </c>
-      <c r="E12" s="9" t="n">
-        <f aca="false">D12-($C$12/6)</f>
-        <v>13.3333333333333</v>
-      </c>
-      <c r="F12" s="9" t="n">
-        <f aca="false">E12-($C$12/6)</f>
-        <v>10</v>
-      </c>
-      <c r="G12" s="9" t="n">
-        <f aca="false">F12-($C$12/6)</f>
-        <v>6.66666666666667</v>
-      </c>
-      <c r="H12" s="9" t="n">
-        <f aca="false">G12-($C$12/6)</f>
-        <v>3.33333333333333</v>
-      </c>
-      <c r="I12" s="9" t="n">
-        <f aca="false">H12-($C$12/6)</f>
+      <c r="C12" s="9">
+        <f>SUM(C2:C9)</f>
+        <v>22</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" ref="D12:I12" si="2">C12-($C$12/6)</f>
+        <v>18.333333333333332</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="2"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="2"/>
+        <v>7.3333333333333339</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="2"/>
+        <v>3.6666666666666674</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update backlog sprint 3 day 6
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -180,13 +180,19 @@
     <t>Design UI Look</t>
   </si>
   <si>
-    <t>Make UI design function</t>
-  </si>
-  <si>
-    <t>Link array to UI</t>
-  </si>
-  <si>
     <t>Android Studio Tutorial</t>
+  </si>
+  <si>
+    <t>Favorites</t>
+  </si>
+  <si>
+    <t>Make UI tab design function</t>
+  </si>
+  <si>
+    <t>Make UI elements</t>
+  </si>
+  <si>
+    <t>Search Activity</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -645,11 +650,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="373346320"/>
-        <c:axId val="373343968"/>
+        <c:axId val="179198232"/>
+        <c:axId val="177919448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373346320"/>
+        <c:axId val="179198232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +671,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="373343968"/>
+        <c:crossAx val="177919448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -674,7 +679,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373343968"/>
+        <c:axId val="177919448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +704,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="373346320"/>
+        <c:crossAx val="179198232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -716,7 +721,6 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -873,25 +877,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,22 +941,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.333333333333332</c:v>
+                  <c:v>15.833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.666666666666666</c:v>
+                  <c:v>12.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>9.5000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3333333333333339</c:v>
+                  <c:v>6.3333333333333357</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6666666666666674</c:v>
+                  <c:v>3.1666666666666692</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -971,11 +975,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="411996032"/>
-        <c:axId val="411999952"/>
+        <c:axId val="177913176"/>
+        <c:axId val="177912784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="411996032"/>
+        <c:axId val="177913176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411999952"/>
+        <c:crossAx val="177912784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="411999952"/>
+        <c:axId val="177912784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,7 +1080,394 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411996032"/>
+        <c:crossAx val="177913176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 3'!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Remaining Hours</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 3'!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Remaining hours</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3333333333333357</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6666666666666692</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="457534752"/>
+        <c:axId val="457535144"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="457534752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457535144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="457535144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457534752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1197,6 +1588,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
@@ -1695,6 +2126,509 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1748,6 +2682,41 @@
       <xdr:colOff>432289</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>89389</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2032,10 +3001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,6 +3246,11 @@
       </c>
       <c r="G10" s="3" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2575,8 +3549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,7 +3605,7 @@
         <v>51</v>
       </c>
       <c r="C2" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
@@ -2648,10 +3622,12 @@
       <c r="H2" s="4">
         <v>1</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
       <c r="J2" s="10">
         <f t="shared" ref="J2:J9" si="0">C2-SUM(D2,E2,F2,G2,H2,I2)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2659,7 +3635,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
@@ -2676,56 +3652,80 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3</v>
+      </c>
       <c r="J3" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
       <c r="J4" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C4-SUM(D4,E4,F4,G4,H4,I4)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
       <c r="G5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
         <v>2</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
       <c r="J5" s="10">
-        <f t="shared" si="0"/>
+        <f>C5-SUM(D5,E5,F5,G5,H5,I5)</f>
         <v>0</v>
       </c>
     </row>
@@ -2795,31 +3795,31 @@
       </c>
       <c r="C11" s="7">
         <f>SUM(C2:C9)</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ref="D11:I11" si="1">C11-SUM(D2:D9)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2828,27 +3828,27 @@
       </c>
       <c r="C12" s="9">
         <f>SUM(C2:C9)</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" ref="D12:I12" si="2">C12-($C$12/6)</f>
-        <v>18.333333333333332</v>
+        <v>15.833333333333334</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="2"/>
-        <v>14.666666666666666</v>
+        <v>12.666666666666668</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>9.5000000000000018</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="2"/>
-        <v>7.3333333333333339</v>
+        <v>6.3333333333333357</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="2"/>
-        <v>3.6666666666666674</v>
+        <v>3.1666666666666692</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="2"/>
@@ -2863,4 +3863,231 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="7">
+        <f>SUM(C2:C9)</f>
+        <v>16</v>
+      </c>
+      <c r="D11" s="7">
+        <f>SUM(D2:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f>SUM(E2:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f>SUM(F2:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <f>SUM(G2:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <f>SUM(H2:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <f>SUM(I2:I9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="9">
+        <f>SUM(C2:C9)</f>
+        <v>16</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" ref="D12:I12" si="0">C12-($C$12/6)</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="0"/>
+        <v>10.666666666666668</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>5.3333333333333357</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666692</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed backlog to show time left for sprint 2
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Estimated Remaining hours</t>
-  </si>
-  <si>
-    <t>Remaining</t>
   </si>
   <si>
     <t>Design UI Look</t>
@@ -650,11 +647,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="179198232"/>
-        <c:axId val="177919448"/>
+        <c:axId val="332787784"/>
+        <c:axId val="332788176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179198232"/>
+        <c:axId val="332787784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +668,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="177919448"/>
+        <c:crossAx val="332788176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -679,7 +676,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177919448"/>
+        <c:axId val="332788176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,7 +701,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="179198232"/>
+        <c:crossAx val="332787784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -975,11 +972,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="177913176"/>
-        <c:axId val="177912784"/>
+        <c:axId val="106394936"/>
+        <c:axId val="106395720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="177913176"/>
+        <c:axId val="106394936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,7 +1018,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177912784"/>
+        <c:crossAx val="106395720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1029,7 +1026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177912784"/>
+        <c:axId val="106395720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177913176"/>
+        <c:crossAx val="106394936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1362,11 +1359,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="457534752"/>
-        <c:axId val="457535144"/>
+        <c:axId val="106397288"/>
+        <c:axId val="334977880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="457534752"/>
+        <c:axId val="106397288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457535144"/>
+        <c:crossAx val="334977880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1416,7 +1413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457535144"/>
+        <c:axId val="334977880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457534752"/>
+        <c:crossAx val="106397288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3549,8 +3546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,9 +3588,7 @@
       <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
@@ -3602,132 +3597,120 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
       </c>
       <c r="D2" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
         <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
       </c>
       <c r="I2" s="4">
         <v>0</v>
       </c>
-      <c r="J2" s="10">
-        <f t="shared" ref="J2:J9" si="0">C2-SUM(D2,E2,F2,G2,H2,I2)</f>
-        <v>0</v>
-      </c>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
       </c>
       <c r="D3" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3</v>
+      </c>
+      <c r="I3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="4">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>3</v>
-      </c>
-      <c r="J3" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="4">
         <v>2</v>
       </c>
       <c r="H4" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
       </c>
-      <c r="J4" s="10">
-        <f>C4-SUM(D4,E4,F4,G4,H4,I4)</f>
-        <v>0</v>
-      </c>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
       </c>
       <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
         <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
       </c>
-      <c r="J5" s="10">
-        <f>C5-SUM(D5,E5,F5,G5,H5,I5)</f>
-        <v>0</v>
-      </c>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -3739,10 +3722,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -3754,10 +3734,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -3769,10 +3746,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -3784,10 +3758,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J9" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -3798,27 +3769,27 @@
         <v>19</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" ref="D11:I11" si="1">C11-SUM(D2:D9)</f>
+        <f>SUM(D2:D9)</f>
         <v>15</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="1"/>
+        <f>SUM(E2:E9)</f>
         <v>15</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="1"/>
+        <f>SUM(F2:F9)</f>
         <v>10</v>
       </c>
       <c r="G11" s="7">
-        <f t="shared" si="1"/>
+        <f>SUM(G2:G9)</f>
         <v>8</v>
       </c>
       <c r="H11" s="7">
-        <f t="shared" si="1"/>
+        <f>SUM(H2:H9)</f>
         <v>3</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="1"/>
+        <f>SUM(I2:I9)</f>
         <v>0</v>
       </c>
     </row>
@@ -3831,27 +3802,27 @@
         <v>19</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" ref="D12:I12" si="2">C12-($C$12/6)</f>
+        <f t="shared" ref="D12:I12" si="0">C12-($C$12/6)</f>
         <v>15.833333333333334</v>
       </c>
       <c r="E12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>12.666666666666668</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>9.5000000000000018</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6.3333333333333357</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.1666666666666692</v>
       </c>
       <c r="I12" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3869,7 +3840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
@@ -3917,7 +3888,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4">
         <v>8</v>
@@ -3935,7 +3906,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4">
         <v>8</v>
@@ -4025,31 +3996,31 @@
         <v>48</v>
       </c>
       <c r="C11" s="7">
-        <f>SUM(C2:C9)</f>
+        <f t="shared" ref="C11:I11" si="0">SUM(C2:C9)</f>
         <v>16</v>
       </c>
       <c r="D11" s="7">
-        <f>SUM(D2:D9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="7">
-        <f>SUM(E2:E9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="7">
-        <f>SUM(F2:F9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G11" s="7">
-        <f>SUM(G2:G9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="7">
-        <f>SUM(H2:H9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I11" s="7">
-        <f>SUM(I2:I9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4062,27 +4033,27 @@
         <v>16</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" ref="D12:I12" si="0">C12-($C$12/6)</f>
+        <f t="shared" ref="D12:I12" si="1">C12-($C$12/6)</f>
         <v>13.333333333333334</v>
       </c>
       <c r="E12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.666666666666668</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0000000000000018</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3333333333333357</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6666666666666692</v>
       </c>
       <c r="I12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sprint 3 day 1
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>as a developer, I want to download android studio, explore, and take tutorial, so I can make a good app</t>
+  </si>
+  <si>
+    <t>Display search results</t>
+  </si>
+  <si>
+    <t>App background service</t>
+  </si>
+  <si>
+    <t>as a developer, I want to have UI elements created so I can use them to make the app look good</t>
   </si>
 </sst>
 </file>
@@ -648,11 +657,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193360168"/>
-        <c:axId val="192746784"/>
+        <c:axId val="82207144"/>
+        <c:axId val="82202832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193360168"/>
+        <c:axId val="82207144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +678,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="192746784"/>
+        <c:crossAx val="82202832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -677,7 +686,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192746784"/>
+        <c:axId val="82202832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +711,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="193360168"/>
+        <c:crossAx val="82207144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -791,7 +800,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -974,11 +982,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="192747960"/>
-        <c:axId val="192747176"/>
+        <c:axId val="82205968"/>
+        <c:axId val="82206360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="192747960"/>
+        <c:axId val="82205968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192747176"/>
+        <c:crossAx val="82206360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1028,7 +1036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192747176"/>
+        <c:axId val="82206360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192747960"/>
+        <c:crossAx val="82205968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1093,7 +1101,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1256,10 +1263,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1326,22 +1333,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.333333333333334</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.666666666666668</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0000000000000018</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3333333333333357</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6666666666666692</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1361,11 +1368,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="192745608"/>
-        <c:axId val="192748352"/>
+        <c:axId val="82200088"/>
+        <c:axId val="82256928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="192745608"/>
+        <c:axId val="82200088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192748352"/>
+        <c:crossAx val="82256928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1415,7 +1422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192748352"/>
+        <c:axId val="82256928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192745608"/>
+        <c:crossAx val="82200088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3002,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,6 +3227,9 @@
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
@@ -3237,11 +3247,17 @@
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>33</v>
@@ -3250,6 +3266,24 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3842,8 +3876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3890,12 +3924,14 @@
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4">
+        <v>8</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -3911,9 +3947,11 @@
         <v>53</v>
       </c>
       <c r="C3" s="4">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -3922,10 +3960,18 @@
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="4">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -3999,11 +4045,11 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:I11" si="0">SUM(C2:C9)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
@@ -4032,27 +4078,27 @@
       </c>
       <c r="C12" s="9">
         <f>SUM(C2:C9)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" ref="D12:I12" si="1">C12-($C$12/6)</f>
-        <v>13.333333333333334</v>
+        <v>15</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>10.666666666666668</v>
+        <v>12</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="1"/>
-        <v>8.0000000000000018</v>
+        <v>9</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="1"/>
-        <v>5.3333333333333357</v>
+        <v>6</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="1"/>
-        <v>2.6666666666666692</v>
+        <v>3</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
sprint 3 day friday
we are awesome.
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Desgin Logo</t>
   </si>
 </sst>
 </file>
@@ -671,11 +674,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="179968200"/>
-        <c:axId val="177078744"/>
+        <c:axId val="238402320"/>
+        <c:axId val="238399184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179968200"/>
+        <c:axId val="238402320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +695,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="177078744"/>
+        <c:crossAx val="238399184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -700,7 +703,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177078744"/>
+        <c:axId val="238399184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +728,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="179968200"/>
+        <c:crossAx val="238402320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -995,11 +998,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="179322792"/>
-        <c:axId val="179325536"/>
+        <c:axId val="238401144"/>
+        <c:axId val="238401536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179322792"/>
+        <c:axId val="238401144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179325536"/>
+        <c:crossAx val="238401536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179325536"/>
+        <c:axId val="238401536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1100,7 +1103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179322792"/>
+        <c:crossAx val="238401144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1276,28 +1279,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1370,49 +1373,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.714285714285715</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.428571428571429</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.142857142857142</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.857142857142856</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.571428571428569</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.285714285714283</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9999999999999964</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.7142857142857109</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.4285714285714253</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.1428571428571397</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8571428571428541</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.5714285714285685</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2857142857142827</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.1086244689504383E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,11 +1432,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="179327888"/>
-        <c:axId val="179326320"/>
+        <c:axId val="240223352"/>
+        <c:axId val="240219824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179327888"/>
+        <c:axId val="240223352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179326320"/>
+        <c:crossAx val="240219824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1483,7 +1486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179326320"/>
+        <c:axId val="240219824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179327888"/>
+        <c:crossAx val="240223352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3071,7 +3074,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3938,7 +3941,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,43 +3973,43 @@
         <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4031,9 +4034,15 @@
       <c r="G2" s="4">
         <v>8</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="4">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4">
+        <v>8</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -4062,11 +4071,17 @@
         <v>5</v>
       </c>
       <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -4097,9 +4112,15 @@
       <c r="G4" s="4">
         <v>5</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5</v>
+      </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -4109,16 +4130,36 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="4">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4">
+        <v>3</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -4209,38 +4250,38 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:I11" si="0">SUM(C2:C9)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:Q11" si="1">SUM(J2:J9)</f>
-        <v>0</v>
+        <f>SUM(J2:J9)</f>
+        <v>18</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K11:Q11" si="1">SUM(K2:K9)</f>
         <v>0</v>
       </c>
       <c r="L11" s="7">
@@ -4274,63 +4315,63 @@
       </c>
       <c r="C12" s="9">
         <f>SUM(C2:C9)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" ref="D12:Q12" si="2">C12-($C$12/14)</f>
-        <v>16.714285714285715</v>
+        <v>19.5</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="2"/>
-        <v>15.428571428571429</v>
+        <v>18</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="2"/>
-        <v>14.142857142857142</v>
+        <v>16.5</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="2"/>
-        <v>12.857142857142856</v>
+        <v>15</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="2"/>
-        <v>11.571428571428569</v>
+        <v>13.5</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="2"/>
-        <v>10.285714285714283</v>
+        <v>12</v>
       </c>
       <c r="J12" s="9">
         <f t="shared" si="2"/>
-        <v>8.9999999999999964</v>
+        <v>10.5</v>
       </c>
       <c r="K12" s="9">
         <f t="shared" si="2"/>
-        <v>7.7142857142857109</v>
+        <v>9</v>
       </c>
       <c r="L12" s="9">
         <f t="shared" si="2"/>
-        <v>6.4285714285714253</v>
+        <v>7.5</v>
       </c>
       <c r="M12" s="9">
         <f t="shared" si="2"/>
-        <v>5.1428571428571397</v>
+        <v>6</v>
       </c>
       <c r="N12" s="9">
         <f t="shared" si="2"/>
-        <v>3.8571428571428541</v>
+        <v>4.5</v>
       </c>
       <c r="O12" s="9">
         <f t="shared" si="2"/>
-        <v>2.5714285714285685</v>
+        <v>3</v>
       </c>
       <c r="P12" s="9">
         <f t="shared" si="2"/>
-        <v>1.2857142857142827</v>
+        <v>1.5</v>
       </c>
       <c r="Q12" s="9">
         <f t="shared" si="2"/>
-        <v>-3.1086244689504383E-15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backlog sprint 3 monday2
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -674,11 +674,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="238402320"/>
-        <c:axId val="238399184"/>
+        <c:axId val="162456552"/>
+        <c:axId val="160507576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238402320"/>
+        <c:axId val="162456552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +695,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="238399184"/>
+        <c:crossAx val="160507576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -703,7 +703,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238399184"/>
+        <c:axId val="160507576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +728,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="238402320"/>
+        <c:crossAx val="162456552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,11 +998,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="238401144"/>
-        <c:axId val="238401536"/>
+        <c:axId val="160514632"/>
+        <c:axId val="160513064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238401144"/>
+        <c:axId val="160514632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,7 +1044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238401536"/>
+        <c:crossAx val="160513064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1052,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238401536"/>
+        <c:axId val="160513064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238401144"/>
+        <c:crossAx val="160514632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1303,13 +1303,13 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1432,11 +1432,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="240223352"/>
-        <c:axId val="240219824"/>
+        <c:axId val="160509928"/>
+        <c:axId val="160509536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="240223352"/>
+        <c:axId val="160509928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240219824"/>
+        <c:crossAx val="160509536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240219824"/>
+        <c:axId val="160509536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,7 +1537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240223352"/>
+        <c:crossAx val="160509928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3940,8 +3940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,9 +4043,15 @@
       <c r="J2" s="4">
         <v>8</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="K2" s="4">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4">
+        <v>8</v>
+      </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -4082,9 +4088,15 @@
       <c r="J3" s="4">
         <v>2</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="K3" s="4">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4">
+        <v>2</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2</v>
+      </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
@@ -4121,9 +4133,15 @@
       <c r="J4" s="4">
         <v>5</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="K4" s="4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5</v>
+      </c>
+      <c r="M4" s="4">
+        <v>5</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
@@ -4160,9 +4178,15 @@
       <c r="J5" s="4">
         <v>3</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+      <c r="M5" s="4">
+        <v>2</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -4282,15 +4306,15 @@
       </c>
       <c r="K11" s="7">
         <f t="shared" ref="K11:Q11" si="1">SUM(K2:K9)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
backlog sprint 3 wednesday
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -674,11 +674,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="162456552"/>
-        <c:axId val="160507576"/>
+        <c:axId val="317237520"/>
+        <c:axId val="315520736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="162456552"/>
+        <c:axId val="317237520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +695,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="160507576"/>
+        <c:crossAx val="315520736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -703,7 +703,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160507576"/>
+        <c:axId val="315520736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +728,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="162456552"/>
+        <c:crossAx val="317237520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,11 +998,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="160514632"/>
-        <c:axId val="160513064"/>
+        <c:axId val="315517992"/>
+        <c:axId val="315518384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="160514632"/>
+        <c:axId val="315517992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,7 +1044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160513064"/>
+        <c:crossAx val="315518384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1052,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160513064"/>
+        <c:axId val="315518384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160514632"/>
+        <c:crossAx val="315517992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1294,28 +1294,28 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1432,11 +1432,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="160509928"/>
-        <c:axId val="160509536"/>
+        <c:axId val="86737312"/>
+        <c:axId val="86738880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="160509928"/>
+        <c:axId val="86737312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160509536"/>
+        <c:crossAx val="86738880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160509536"/>
+        <c:axId val="86738880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,7 +1537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160509928"/>
+        <c:crossAx val="86737312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3940,8 +3940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4035,25 +4035,29 @@
         <v>8</v>
       </c>
       <c r="H2" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K2" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L2" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M2" s="4">
-        <v>8</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="N2" s="4">
+        <v>5</v>
+      </c>
+      <c r="O2" s="4">
+        <v>5</v>
+      </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
@@ -4097,8 +4101,12 @@
       <c r="M3" s="4">
         <v>2</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="N3" s="4">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2</v>
+      </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
@@ -4142,8 +4150,12 @@
       <c r="M4" s="4">
         <v>5</v>
       </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="N4" s="4">
+        <v>5</v>
+      </c>
+      <c r="O4" s="4">
+        <v>3</v>
+      </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
@@ -4187,8 +4199,12 @@
       <c r="M5" s="4">
         <v>2</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="N5" s="4">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
@@ -4294,35 +4310,35 @@
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="7">
         <f>SUM(J2:J9)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ref="K11:Q11" si="1">SUM(K2:K9)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P11" s="7">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Updated Backlog and added BackgroundService
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\TVTrackr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elijah\Documents\GitHub\TVTrackr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="992" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,7 +430,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -549,6 +549,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-54EF-4855-BF38-8DF268E1E09A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -634,6 +639,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-54EF-4855-BF38-8DF268E1E09A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -656,6 +666,11 @@
             </c:spPr>
           </c:marker>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-54EF-4855-BF38-8DF268E1E09A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -777,7 +792,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -924,6 +939,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F843-4653-B083-E41C495DA750}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -988,6 +1008,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F843-4653-B083-E41C495DA750}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1184,7 +1209,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1198,7 +1223,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1327,6 +1351,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91E4-4DE7-A8A8-AE610BC285AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1421,6 +1450,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-91E4-4DE7-A8A8-AE610BC285AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1551,7 +1585,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2720,7 +2753,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2755,7 +2794,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2790,7 +2835,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2884,6 +2935,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2919,6 +2987,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3077,21 +3162,21 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="15.28515625"/>
-    <col min="4" max="4" width="18.5703125"/>
-    <col min="5" max="5" width="8.5703125"/>
-    <col min="6" max="6" width="12.5703125"/>
-    <col min="7" max="7" width="26.42578125"/>
+    <col min="1" max="1" width="8.6640625"/>
+    <col min="2" max="2" width="16.88671875"/>
+    <col min="3" max="3" width="15.33203125"/>
+    <col min="4" max="4" width="18.5546875"/>
+    <col min="5" max="5" width="8.5546875"/>
+    <col min="6" max="6" width="12.5546875"/>
+    <col min="7" max="7" width="26.44140625"/>
     <col min="8" max="8" width="11"/>
-    <col min="9" max="9" width="17.5703125"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="9" max="9" width="17.5546875"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3117,7 +3202,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3140,7 +3225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3164,7 +3249,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3188,7 +3273,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3212,7 +3297,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3236,7 +3321,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3260,7 +3345,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3284,7 +3369,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3304,7 +3389,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3327,7 +3412,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3364,17 +3449,17 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125"/>
-    <col min="2" max="2" width="30.85546875"/>
-    <col min="3" max="3" width="14.7109375"/>
-    <col min="4" max="4" width="8.7109375"/>
-    <col min="5" max="5" width="17.42578125"/>
-    <col min="6" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="12.44140625"/>
+    <col min="2" max="2" width="30.88671875"/>
+    <col min="3" max="3" width="14.6640625"/>
+    <col min="4" max="4" width="8.6640625"/>
+    <col min="5" max="5" width="17.44140625"/>
+    <col min="6" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3406,7 +3491,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3435,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3464,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3493,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3522,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3533,7 +3618,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3544,7 +3629,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3555,7 +3640,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3566,7 +3651,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -3599,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
@@ -3632,9 +3717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3650,17 +3735,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125"/>
-    <col min="2" max="2" width="30.85546875"/>
-    <col min="3" max="3" width="14.7109375"/>
-    <col min="4" max="4" width="8.7109375"/>
-    <col min="5" max="5" width="17.42578125"/>
-    <col min="6" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="12.44140625"/>
+    <col min="2" max="2" width="30.88671875"/>
+    <col min="3" max="3" width="14.6640625"/>
+    <col min="4" max="4" width="8.6640625"/>
+    <col min="5" max="5" width="17.44140625"/>
+    <col min="6" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3692,7 +3777,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>7</v>
       </c>
@@ -3722,7 +3807,7 @@
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>4</v>
       </c>
@@ -3752,7 +3837,7 @@
       </c>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>6</v>
       </c>
@@ -3782,7 +3867,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3812,7 +3897,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3824,7 +3909,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3836,7 +3921,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3848,7 +3933,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3860,7 +3945,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -3893,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
@@ -3926,9 +4011,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3941,25 +4026,25 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.5546875" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="12" width="3.28515625" customWidth="1"/>
-    <col min="13" max="14" width="3.5703125" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="8" max="9" width="2.88671875" customWidth="1"/>
+    <col min="10" max="12" width="3.33203125" customWidth="1"/>
+    <col min="13" max="14" width="3.5546875" customWidth="1"/>
+    <col min="15" max="15" width="2.88671875" customWidth="1"/>
+    <col min="16" max="16" width="3.33203125" customWidth="1"/>
     <col min="17" max="17" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -4012,7 +4097,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>10</v>
       </c>
@@ -4061,7 +4146,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -4110,7 +4195,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>9</v>
       </c>
@@ -4156,10 +4241,12 @@
       <c r="O4" s="4">
         <v>3</v>
       </c>
-      <c r="P4" s="4"/>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -4208,7 +4295,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -4227,7 +4314,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4246,7 +4333,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4265,7 +4352,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4284,7 +4371,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -4349,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update backlog sprint 3 friday2
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elijah\Documents\GitHub\TVTrackr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\TVTrackr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="992" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,7 +430,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -512,7 +512,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -549,7 +549,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-54EF-4855-BF38-8DF268E1E09A}"/>
             </c:ext>
@@ -602,7 +602,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -639,7 +639,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-54EF-4855-BF38-8DF268E1E09A}"/>
             </c:ext>
@@ -666,7 +666,7 @@
             </c:spPr>
           </c:marker>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-54EF-4855-BF38-8DF268E1E09A}"/>
             </c:ext>
@@ -689,11 +689,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="317237520"/>
-        <c:axId val="315520736"/>
+        <c:axId val="320813432"/>
+        <c:axId val="319265576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="317237520"/>
+        <c:axId val="320813432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +710,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="315520736"/>
+        <c:crossAx val="319265576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -718,7 +718,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="315520736"/>
+        <c:axId val="319265576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +743,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="317237520"/>
+        <c:crossAx val="320813432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -792,7 +792,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -939,7 +939,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F843-4653-B083-E41C495DA750}"/>
             </c:ext>
@@ -1008,7 +1008,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F843-4653-B083-E41C495DA750}"/>
             </c:ext>
@@ -1023,11 +1023,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="315517992"/>
-        <c:axId val="315518384"/>
+        <c:axId val="319271848"/>
+        <c:axId val="319272632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="315517992"/>
+        <c:axId val="319271848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1069,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315518384"/>
+        <c:crossAx val="319272632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="315518384"/>
+        <c:axId val="319272632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315517992"/>
+        <c:crossAx val="319271848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1209,7 +1209,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1223,6 +1223,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1342,16 +1343,16 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-91E4-4DE7-A8A8-AE610BC285AA}"/>
             </c:ext>
@@ -1450,7 +1451,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-91E4-4DE7-A8A8-AE610BC285AA}"/>
             </c:ext>
@@ -1466,11 +1467,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86737312"/>
-        <c:axId val="86738880"/>
+        <c:axId val="319266752"/>
+        <c:axId val="319267144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86737312"/>
+        <c:axId val="319266752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1513,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86738880"/>
+        <c:crossAx val="319267144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1520,7 +1521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86738880"/>
+        <c:axId val="319267144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1572,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86737312"/>
+        <c:crossAx val="319266752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1585,6 +1586,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2756,7 +2758,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2797,7 +2799,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2838,7 +2840,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2935,23 +2937,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2987,23 +2972,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3162,21 +3130,21 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625"/>
-    <col min="2" max="2" width="16.88671875"/>
-    <col min="3" max="3" width="15.33203125"/>
-    <col min="4" max="4" width="18.5546875"/>
-    <col min="5" max="5" width="8.5546875"/>
-    <col min="6" max="6" width="12.5546875"/>
-    <col min="7" max="7" width="26.44140625"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="15.28515625"/>
+    <col min="4" max="4" width="18.5703125"/>
+    <col min="5" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="12.5703125"/>
+    <col min="7" max="7" width="26.42578125"/>
     <col min="8" max="8" width="11"/>
-    <col min="9" max="9" width="17.5546875"/>
-    <col min="10" max="1025" width="8.6640625"/>
+    <col min="9" max="9" width="17.5703125"/>
+    <col min="10" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3202,7 +3170,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3225,7 +3193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3249,7 +3217,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3273,7 +3241,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3297,7 +3265,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3321,7 +3289,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3345,7 +3313,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3369,7 +3337,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3389,7 +3357,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3412,7 +3380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3449,17 +3417,17 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625"/>
-    <col min="2" max="2" width="30.88671875"/>
-    <col min="3" max="3" width="14.6640625"/>
-    <col min="4" max="4" width="8.6640625"/>
-    <col min="5" max="5" width="17.44140625"/>
-    <col min="6" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="12.42578125"/>
+    <col min="2" max="2" width="30.85546875"/>
+    <col min="3" max="3" width="14.7109375"/>
+    <col min="4" max="4" width="8.7109375"/>
+    <col min="5" max="5" width="17.42578125"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3491,7 +3459,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3520,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3549,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3578,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3607,7 +3575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3618,7 +3586,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3629,7 +3597,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3640,7 +3608,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3651,7 +3619,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -3684,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
@@ -3717,9 +3685,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3735,17 +3703,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625"/>
-    <col min="2" max="2" width="30.88671875"/>
-    <col min="3" max="3" width="14.6640625"/>
-    <col min="4" max="4" width="8.6640625"/>
-    <col min="5" max="5" width="17.44140625"/>
-    <col min="6" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="12.42578125"/>
+    <col min="2" max="2" width="30.85546875"/>
+    <col min="3" max="3" width="14.7109375"/>
+    <col min="4" max="4" width="8.7109375"/>
+    <col min="5" max="5" width="17.42578125"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3777,7 +3745,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>7</v>
       </c>
@@ -3807,7 +3775,7 @@
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>4</v>
       </c>
@@ -3837,7 +3805,7 @@
       </c>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>6</v>
       </c>
@@ -3867,7 +3835,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3897,7 +3865,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3909,7 +3877,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3921,7 +3889,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3933,7 +3901,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3945,7 +3913,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -3978,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
@@ -4011,9 +3979,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4025,26 +3993,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="2.5546875" customWidth="1"/>
-    <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="9" width="2.88671875" customWidth="1"/>
-    <col min="10" max="12" width="3.33203125" customWidth="1"/>
-    <col min="13" max="14" width="3.5546875" customWidth="1"/>
-    <col min="15" max="15" width="2.88671875" customWidth="1"/>
-    <col min="16" max="16" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="7" width="3" customWidth="1"/>
+    <col min="8" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="12" width="3.28515625" customWidth="1"/>
+    <col min="13" max="14" width="3.5703125" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
     <col min="17" max="17" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -4097,7 +4063,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>10</v>
       </c>
@@ -4143,10 +4109,14 @@
       <c r="O2" s="4">
         <v>5</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="P2" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -4192,10 +4162,14 @@
       <c r="O3" s="4">
         <v>2</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="P3" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>9</v>
       </c>
@@ -4244,9 +4218,11 @@
       <c r="P4" s="4">
         <v>0</v>
       </c>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -4292,10 +4268,14 @@
       <c r="O5" s="4">
         <v>1</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -4314,7 +4294,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4333,7 +4313,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4352,7 +4332,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4371,7 +4351,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -4429,14 +4409,14 @@
       </c>
       <c r="P11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
added sprint 4 to backlog
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -16,13 +16,14 @@
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -114,9 +115,6 @@
     <t>Calendar</t>
   </si>
   <si>
-    <t>Future</t>
-  </si>
-  <si>
     <t>as a customer, I want to have a calandar so I can see what's going on in the future</t>
   </si>
   <si>
@@ -217,6 +215,18 @@
   </si>
   <si>
     <t>Desgin Logo</t>
+  </si>
+  <si>
+    <t>Logo Design Compatability</t>
+  </si>
+  <si>
+    <t>Productionalize Search Functionality</t>
+  </si>
+  <si>
+    <t>Connect notifications and favorites</t>
+  </si>
+  <si>
+    <t>Calender</t>
   </si>
 </sst>
 </file>
@@ -689,11 +699,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="320813432"/>
-        <c:axId val="319265576"/>
+        <c:axId val="96076184"/>
+        <c:axId val="94882568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="320813432"/>
+        <c:axId val="96076184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +720,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="319265576"/>
+        <c:crossAx val="94882568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -718,7 +728,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319265576"/>
+        <c:axId val="94882568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +753,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="320813432"/>
+        <c:crossAx val="96076184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1023,11 +1033,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="319271848"/>
-        <c:axId val="319272632"/>
+        <c:axId val="94883352"/>
+        <c:axId val="94883744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319271848"/>
+        <c:axId val="94883352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319272632"/>
+        <c:crossAx val="94883744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319272632"/>
+        <c:axId val="94883744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319271848"/>
+        <c:crossAx val="94883352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1467,11 +1477,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="319266752"/>
-        <c:axId val="319267144"/>
+        <c:axId val="94885704"/>
+        <c:axId val="94887272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319266752"/>
+        <c:axId val="94885704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1513,7 +1523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319267144"/>
+        <c:crossAx val="94887272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1521,7 +1531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319267144"/>
+        <c:axId val="94887272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319266752"/>
+        <c:crossAx val="94885704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3127,7 +3137,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3261,7 +3271,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -3309,7 +3319,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -3330,7 +3340,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>28</v>
@@ -3350,11 +3360,14 @@
       <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
       <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3362,7 +3375,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
@@ -3377,7 +3390,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3385,7 +3398,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>25</v>
@@ -3400,7 +3413,7 @@
         <v>22</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3429,31 +3442,31 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -3464,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4">
         <v>2</v>
@@ -3493,7 +3506,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4">
         <v>6</v>
@@ -3522,7 +3535,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
@@ -3621,7 +3634,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="7">
         <f>SUM(C2:C9)</f>
@@ -3654,7 +3667,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="9">
         <f>SUM(C2:C9)</f>
@@ -3715,31 +3728,31 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -3750,7 +3763,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
@@ -3780,7 +3793,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
@@ -3810,7 +3823,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
@@ -3840,7 +3853,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -3915,7 +3928,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:I11" si="0">SUM(C2:C9)</f>
@@ -3948,7 +3961,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="9">
         <f>SUM(C2:C9)</f>
@@ -3993,8 +4006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4002,65 +4015,65 @@
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="7" width="3" customWidth="1"/>
-    <col min="8" max="9" width="2.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
     <col min="10" max="12" width="3.28515625" customWidth="1"/>
-    <col min="13" max="14" width="3.5703125" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="13" max="15" width="3.5703125" customWidth="1"/>
     <col min="16" max="16" width="3.28515625" customWidth="1"/>
     <col min="17" max="17" width="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4068,7 +4081,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4">
         <v>8</v>
@@ -4121,7 +4134,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4">
         <v>5</v>
@@ -4174,7 +4187,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4">
         <v>5</v>
@@ -4227,7 +4240,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
@@ -4353,7 +4366,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:I11" si="0">SUM(C2:C9)</f>
@@ -4418,7 +4431,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="9">
         <f>SUM(C2:C9)</f>
@@ -4485,4 +4498,387 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" ref="C11:I11" si="0">SUM(C2:C9)</f>
+        <v>18</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f>SUM(J2:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" ref="K11:Q11" si="1">SUM(K2:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="9">
+        <f>SUM(C2:C9)</f>
+        <v>18</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" ref="D12:P12" si="2">C12-($C$12/14)</f>
+        <v>16.714285714285715</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="2"/>
+        <v>15.428571428571429</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="2"/>
+        <v>14.142857142857142</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="2"/>
+        <v>12.857142857142856</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="2"/>
+        <v>11.571428571428569</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="2"/>
+        <v>10.285714285714283</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="2"/>
+        <v>8.9999999999999964</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="2"/>
+        <v>7.7142857142857109</v>
+      </c>
+      <c r="L12" s="9">
+        <f t="shared" si="2"/>
+        <v>6.4285714285714253</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="2"/>
+        <v>5.1428571428571397</v>
+      </c>
+      <c r="N12" s="9">
+        <f t="shared" si="2"/>
+        <v>3.8571428571428541</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="2"/>
+        <v>2.5714285714285685</v>
+      </c>
+      <c r="P12" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2857142857142827</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sprinty 4 day monday1
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -699,11 +699,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96076184"/>
-        <c:axId val="94882568"/>
+        <c:axId val="184498112"/>
+        <c:axId val="182826960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96076184"/>
+        <c:axId val="184498112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +720,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="94882568"/>
+        <c:crossAx val="182826960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -728,7 +728,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94882568"/>
+        <c:axId val="182826960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +753,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96076184"/>
+        <c:crossAx val="184498112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1033,11 +1033,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="94883352"/>
-        <c:axId val="94883744"/>
+        <c:axId val="182821472"/>
+        <c:axId val="182825392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94883352"/>
+        <c:axId val="182821472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94883744"/>
+        <c:crossAx val="182825392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1087,7 +1087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94883744"/>
+        <c:axId val="182825392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94883352"/>
+        <c:crossAx val="182821472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1477,11 +1477,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94885704"/>
-        <c:axId val="94887272"/>
+        <c:axId val="85984752"/>
+        <c:axId val="85983184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94885704"/>
+        <c:axId val="85984752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94887272"/>
+        <c:crossAx val="85983184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1531,7 +1531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94887272"/>
+        <c:axId val="85983184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94885704"/>
+        <c:crossAx val="85984752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2768,7 +2768,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,7 +2809,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2850,7 +2850,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4006,7 +4006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4504,8 +4504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4577,9 +4577,15 @@
       <c r="C2" s="4">
         <v>4</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="4">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -4602,9 +4608,15 @@
       <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -4627,9 +4639,15 @@
       <c r="C4" s="4">
         <v>4</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -4652,9 +4670,15 @@
       <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -4677,9 +4701,15 @@
       <c r="C6" s="4">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="4">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -4759,15 +4789,15 @@
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updated Spring log for Elijah 11/09
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\TVTrackr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elijah\Documents\GitHub\TVTrackr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
     <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,7 +440,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -522,7 +522,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -559,7 +559,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-54EF-4855-BF38-8DF268E1E09A}"/>
             </c:ext>
@@ -612,7 +612,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -649,7 +649,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-54EF-4855-BF38-8DF268E1E09A}"/>
             </c:ext>
@@ -676,7 +676,7 @@
             </c:spPr>
           </c:marker>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-54EF-4855-BF38-8DF268E1E09A}"/>
             </c:ext>
@@ -802,7 +802,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -949,7 +949,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F843-4653-B083-E41C495DA750}"/>
             </c:ext>
@@ -1018,7 +1018,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F843-4653-B083-E41C495DA750}"/>
             </c:ext>
@@ -1219,7 +1219,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1233,7 +1233,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1362,7 +1361,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-91E4-4DE7-A8A8-AE610BC285AA}"/>
             </c:ext>
@@ -1461,7 +1460,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-91E4-4DE7-A8A8-AE610BC285AA}"/>
             </c:ext>
@@ -1596,7 +1595,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2768,7 +2766,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,7 +2807,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2850,7 +2848,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2947,6 +2945,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2982,6 +2997,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4505,7 +4537,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,8 +4711,12 @@
       <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -4801,11 +4837,11 @@
       </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
sprinty last day friesday
</commit_message>
<xml_diff>
--- a/TvTrackrBacklog.xlsx
+++ b/TvTrackrBacklog.xlsx
@@ -699,11 +699,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184498112"/>
-        <c:axId val="182826960"/>
+        <c:axId val="181448408"/>
+        <c:axId val="179830256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184498112"/>
+        <c:axId val="181448408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +720,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="182826960"/>
+        <c:crossAx val="179830256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -728,7 +728,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182826960"/>
+        <c:axId val="179830256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +753,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="184498112"/>
+        <c:crossAx val="181448408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1033,11 +1033,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="182821472"/>
-        <c:axId val="182825392"/>
+        <c:axId val="179825552"/>
+        <c:axId val="179829080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182821472"/>
+        <c:axId val="179825552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182825392"/>
+        <c:crossAx val="179829080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1087,7 +1087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182825392"/>
+        <c:axId val="179829080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182821472"/>
+        <c:crossAx val="179825552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1233,7 +1233,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1477,11 +1476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85984752"/>
-        <c:axId val="85983184"/>
+        <c:axId val="179829472"/>
+        <c:axId val="179822808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85984752"/>
+        <c:axId val="179829472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85983184"/>
+        <c:crossAx val="179822808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1531,7 +1530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85983184"/>
+        <c:axId val="179822808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85984752"/>
+        <c:crossAx val="179829472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1596,7 +1595,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2768,7 +2766,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,7 +2807,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2850,7 +2848,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4505,7 +4503,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,10 +4584,18 @@
       <c r="F2" s="4">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3</v>
+      </c>
+      <c r="J2" s="4">
+        <v>3</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -4617,10 +4623,18 @@
       <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -4648,10 +4662,18 @@
       <c r="F4" s="4">
         <v>4</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="G4" s="4">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4">
+        <v>4</v>
+      </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -4679,10 +4701,18 @@
       <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -4710,10 +4740,18 @@
       <c r="F6" s="4">
         <v>6</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -4801,19 +4839,19 @@
       </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J11" s="7">
         <f>SUM(J2:J9)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ref="K11:Q11" si="1">SUM(K2:K9)</f>

</xml_diff>